<commit_message>
Dodano wyniki dla incremental test ze wstepnym wykresem by zobaczyc jak wyszlo
</commit_message>
<xml_diff>
--- a/doc/res/wynikiBenchmarkow.xlsx
+++ b/doc/res/wynikiBenchmarkow.xlsx
@@ -4,24 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="test 2D" sheetId="1" r:id="rId1"/>
     <sheet name="test 3D" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="test incrementalObjects" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>Benchmark</t>
-  </si>
-  <si>
-    <t>Telefon</t>
   </si>
   <si>
     <t>S4</t>
@@ -40,6 +37,9 @@
   </si>
   <si>
     <t>iPad 1</t>
+  </si>
+  <si>
+    <t>Device</t>
   </si>
 </sst>
 </file>
@@ -90,6 +90,700 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia 625</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$G$3:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="45778048"/>
+        <c:axId val="45779584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="45778048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="2700000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45779584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="45779584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="45778048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,7 +1076,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="F7" sqref="F7:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,25 +1090,25 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -821,33 +1515,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1252,12 +1944,332 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1">
+        <v>56</v>
+      </c>
+      <c r="C3" s="1">
+        <v>58</v>
+      </c>
+      <c r="D3" s="1">
+        <v>59</v>
+      </c>
+      <c r="E3" s="1">
+        <v>59</v>
+      </c>
+      <c r="F3" s="1">
+        <v>59</v>
+      </c>
+      <c r="G3" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1">
+        <v>53</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44</v>
+      </c>
+      <c r="D4" s="1">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1">
+        <v>58</v>
+      </c>
+      <c r="F4" s="1">
+        <v>58</v>
+      </c>
+      <c r="G4" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>250</v>
+      </c>
+      <c r="B5" s="1">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1">
+        <v>37</v>
+      </c>
+      <c r="E5" s="1">
+        <v>58</v>
+      </c>
+      <c r="F5" s="1">
+        <v>51</v>
+      </c>
+      <c r="G5" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>500</v>
+      </c>
+      <c r="B6" s="1">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>750</v>
+      </c>
+      <c r="B7" s="1">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1250</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1500</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>6</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1750</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Stworzono wykresy i wykresy porownawcze (brakuje testu tworzenia obiektow!), edytowano styl dodajac justowanie, stworzono dzial "benchmark" do ktorego wrzuono wyniki wraz z krotkimi wnioskami
</commit_message>
<xml_diff>
--- a/doc/res/wynikiBenchmarkow.xlsx
+++ b/doc/res/wynikiBenchmarkow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test 2D" sheetId="1" r:id="rId1"/>
@@ -16,15 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>Benchmark</t>
   </si>
   <si>
     <t>S4</t>
-  </si>
-  <si>
-    <t>Lumia 625</t>
   </si>
   <si>
     <t>Core</t>
@@ -40,6 +37,21 @@
   </si>
   <si>
     <t>Device</t>
+  </si>
+  <si>
+    <t>Lumia</t>
+  </si>
+  <si>
+    <t>Róznica pomiedzy ruchomymi a nieruchomymi</t>
+  </si>
+  <si>
+    <t>Obiekty</t>
+  </si>
+  <si>
+    <t>Flops</t>
+  </si>
+  <si>
+    <t>Roznica pomiedzy 2D a3D</t>
   </si>
 </sst>
 </file>
@@ -75,9 +87,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -106,18 +119,55 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200"/>
+              <a:t>Test obiektów nieruchomych</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17965266841644795"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13216907261592301"/>
+          <c:y val="0.19491907261592301"/>
+          <c:w val="0.69860979877515306"/>
+          <c:h val="0.66595290172061827"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'test incrementalObjects'!$B$2</c:f>
+              <c:f>'test 2D'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -126,186 +176,102 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+              <c:f>'test 2D'!$I$4:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1750</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$B$3:$B$12</c:f>
+              <c:f>'test 2D'!$B$4:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>58.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'test incrementalObjects'!$C$1</c:f>
+              <c:f>'test 2D'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Lumia 625</c:v>
+                  <c:v>Lumia</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+              <c:f>'test 2D'!$I$4:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1750</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$C$3:$C$12</c:f>
+              <c:f>'test 2D'!$C$4:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>57.55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'test incrementalObjects'!$D$1</c:f>
+              <c:f>'test 2D'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -314,92 +280,50 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+              <c:f>'test 2D'!$I$4:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1750</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$D$3:$D$12</c:f>
+              <c:f>'test 2D'!$D$4:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>58.21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'test incrementalObjects'!$E$1</c:f>
+              <c:f>'test 2D'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -408,92 +332,50 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+              <c:f>'test 2D'!$I$4:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1750</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$E$3:$E$12</c:f>
+              <c:f>'test 2D'!$E$4:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>58.440886473217603</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.828164061085673</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.49078268317411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'test incrementalObjects'!$F$1</c:f>
+              <c:f>'test 2D'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -502,92 +384,50 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+              <c:f>'test 2D'!$I$4:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1750</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$F$3:$F$12</c:f>
+              <c:f>'test 2D'!$F$4:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>57.69229657050662</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.655811199707436</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.875839752131377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'test incrementalObjects'!$G$1</c:f>
+              <c:f>'test 2D'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -596,85 +436,43 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+              <c:f>'test 2D'!$I$4:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1250</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1750</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'test incrementalObjects'!$G$3:$G$12</c:f>
+              <c:f>'test 2D'!$G$4:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>57.175167463545776</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.438872948705843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.901683159318985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -684,33 +482,41 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="45778048"/>
-        <c:axId val="45779584"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="153858816"/>
+        <c:axId val="153860736"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="45778048"/>
+        <c:axId val="153858816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Ilość obiektów</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr rot="2700000"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="45779584"/>
+        <c:crossAx val="153860736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -718,18 +524,44 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45779584"/>
+        <c:axId val="153860736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>FPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.208223972003499E-3"/>
+              <c:y val="0.49170312044327791"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45778048"/>
+        <c:crossAx val="153858816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -751,20 +583,2830 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200"/>
+              <a:t>Różnica</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+              <a:t> pomiędzy testami obiektów nieruchomych a ruchomych</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL" sz="1200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12113188976377953"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 2D'!$I$8:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 2D'!$B$25:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.58999999999999631</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.259999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 2D'!$I$8:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 2D'!$C$25:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3600000000000012</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 2D'!$I$8:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 2D'!$D$25:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.0000000000003126E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.1199999999999974</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.870000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 2D'!$I$8:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 2D'!$E$25:$E$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.22905643082614091</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.38532410907959047</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.415285218337871</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 2D'!$I$8:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 2D'!$F$25:$F$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4890051564393119</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.486747140225404</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 2D'!$I$8:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 2D'!$G$25:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.496253814651205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5497353439164989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="154569728"/>
+        <c:axId val="154580096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="154569728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Ilość obiektów</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.36499453193350834"/>
+              <c:y val="0.92960629921259841"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154580096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="154580096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>FPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154569728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200"/>
+              <a:t>Test obiektów ruchomych ze</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+              <a:t> sztucznymi operacjami zmiennoprzecinkowymi</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13445822397200349"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13551640419947505"/>
+          <c:y val="0.15001166520851561"/>
+          <c:w val="0.67966491688538933"/>
+          <c:h val="0.68676290463692036"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('test 2D'!$B$13,'test 2D'!$B$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>55.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('test 2D'!$C$13,'test 2D'!$C$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>44.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('test 2D'!$D$13,'test 2D'!$D$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>54.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('test 2D'!$E$13,'test 2D'!$E$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>58.544740126178375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.898070846558838</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('test 2D'!$F$13,'test 2D'!$F$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>58.514229187787393</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.395496836868404</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 2D'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('test 2D'!$G$13,'test 2D'!$G$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>57.280888346165227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.083496922929051</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="154678784"/>
+        <c:axId val="154680704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="154678784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Operacje</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> zmiennoprzecinkowe na sekundę</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.23400853018372703"/>
+              <c:y val="0.92960629921259841"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154680704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="154680704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="40"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>FPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.7777777777777779E-3"/>
+              <c:y val="0.45951552930883638"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154678784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200"/>
+              <a:t>Różnica pomiędzy testami dwu i trójwymiarowymi dla obiektów nieruchomych</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10945822397200351"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13789129483814525"/>
+          <c:y val="0.17315981335666372"/>
+          <c:w val="0.68991535433070861"/>
+          <c:h val="0.72914333624963545"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$B$23:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-0.60000000000000142</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.2000000000000028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69999999999999929</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$C$23:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-1.4500000000000028</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30000000000000071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$D$23:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-0.78999999999999915</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.7700000000000031</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.4699999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$E$23:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-0.89346417363342567</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.36183593891432508</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.5833581553526912</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$F$23:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-1.647703429493383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.985732995172377</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.0516182310616387</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$G$23:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-2.6453525710801529</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.0260051402627326</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.9147222144532137</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="90826240"/>
+        <c:axId val="90915200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90826240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Ilość obiektów</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90915200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90915200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>FPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90826240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.83613998250218724"/>
+          <c:y val="0.26343175853018369"/>
+          <c:w val="0.14592979002624673"/>
+          <c:h val="0.50230314960629918"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200"/>
+              <a:t>Różnica pomiędzy testami dwu i trójwymiarowymi dla obiektów ruchomych</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10945822397200351"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13789129483814525"/>
+          <c:y val="0.17315981335666372"/>
+          <c:w val="0.68991535433070861"/>
+          <c:h val="0.72914333624963545"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$B$27:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-1.1899999999999977</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6999999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$C$27:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-1.2199999999999989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.6099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9399999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$D$27:$D$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-0.81000000000000227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$E$27:$E$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-1.4481699576085347</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.79504474814535797</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.4467728867867748</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$F$27:$F$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-0.68615128226476685</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.6703326216909602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.5933933051923717</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test 3D'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test 3D'!$H$4:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test 3D'!$G$27:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-0.9746497500343807</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.2799295639652897</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.9260039479109636</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="91073920"/>
+        <c:axId val="89769088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="91073920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Ilość obiektów</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89769088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="89769088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>FPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91073920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.83613998250218724"/>
+          <c:y val="0.26343175853018369"/>
+          <c:w val="0.16386001749781276"/>
+          <c:h val="0.50230314960629918"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200"/>
+              <a:t>Test inkrementalny</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.36286111111111113"/>
+          <c:y val="0"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16607195975503061"/>
+          <c:y val="8.6817220764071154E-2"/>
+          <c:w val="0.62568394575678044"/>
+          <c:h val="0.71863662875473888"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test incrementalObjects'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test incrementalObjects'!$G$3:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="154780032"/>
+        <c:axId val="154781568"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="154780032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Ilość obiektów</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.3785667104111986"/>
+              <c:y val="0.92960629921259841"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="2700000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="154781568"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="154781568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>FPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.7777777777777779E-3"/>
+              <c:y val="0.40068387284922719"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="154780032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.81791601049868767"/>
+          <c:y val="0.22026027996500441"/>
+          <c:w val="0.18208398950131233"/>
+          <c:h val="0.50230314960629918"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Wykres 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Wykres 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1073,10 +3715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:G10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,25 +3732,31 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1164,6 +3812,9 @@
       <c r="G4" s="1">
         <v>57.175167463545776</v>
       </c>
+      <c r="I4" s="2">
+        <v>50</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1190,6 +3841,9 @@
       <c r="G5" s="1">
         <v>39.438872948705843</v>
       </c>
+      <c r="I5" s="2">
+        <v>250</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -1216,6 +3870,9 @@
       <c r="G6" s="1">
         <v>24.901683159318985</v>
       </c>
+      <c r="I6" s="2">
+        <v>500</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1242,6 +3899,7 @@
       <c r="G7" s="1">
         <v>58.637344926509151</v>
       </c>
+      <c r="I7" s="2"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -1268,6 +3926,9 @@
       <c r="G8" s="1">
         <v>58.715350249965617</v>
       </c>
+      <c r="I8" s="2">
+        <v>50</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -1294,6 +3955,9 @@
       <c r="G9" s="1">
         <v>28.942619134054638</v>
       </c>
+      <c r="I9" s="2">
+        <v>250</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1320,6 +3984,9 @@
       <c r="G10" s="1">
         <v>15.351947815402486</v>
       </c>
+      <c r="I10" s="2">
+        <v>500</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -1346,6 +4013,7 @@
       <c r="G11" s="1">
         <v>57.784885697301512</v>
       </c>
+      <c r="I11" s="2"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -1372,6 +4040,9 @@
       <c r="G12" s="1">
         <v>57.528573776787539</v>
       </c>
+      <c r="I12" s="2">
+        <v>100</v>
+      </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -1398,6 +4069,12 @@
       <c r="G13" s="1">
         <v>57.280888346165227</v>
       </c>
+      <c r="I13" s="2">
+        <v>100</v>
+      </c>
+      <c r="J13" s="1">
+        <v>225</v>
+      </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1424,6 +4101,9 @@
       <c r="G14" s="1">
         <v>57.071326837826049</v>
       </c>
+      <c r="I14" s="2">
+        <v>100</v>
+      </c>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -1450,6 +4130,9 @@
       <c r="G15" s="1">
         <v>56.405065100646631</v>
       </c>
+      <c r="I15" s="2">
+        <v>100</v>
+      </c>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -1476,6 +4159,9 @@
       <c r="G16" s="1">
         <v>53.665230666043463</v>
       </c>
+      <c r="I16" s="2">
+        <v>100</v>
+      </c>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
@@ -1502,44 +4188,133 @@
       <c r="G17" s="1">
         <v>48.083496922929051</v>
       </c>
+      <c r="I17" s="2">
+        <v>100</v>
+      </c>
+      <c r="J17" s="1">
+        <v>2500</v>
+      </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <f>B4-B8</f>
+        <v>0.58999999999999631</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25:E25" si="0">D4-D8</f>
+        <v>2.0000000000003126E-2</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.22905643082614091</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <f t="shared" ref="B26:G27" si="1">B5-B9</f>
+        <v>12.259999999999998</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="1"/>
+        <v>8.14</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="1"/>
+        <v>9.1199999999999974</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38532410907959047</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="1"/>
+        <v>7.4890051564393119</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="1"/>
+        <v>10.496253814651205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="1"/>
+        <v>3.3600000000000012</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="1"/>
+        <v>4.870000000000001</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>17.415285218337871</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="1"/>
+        <v>17.486747140225404</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="1"/>
+        <v>9.5497353439164989</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1595,6 +4370,9 @@
       <c r="G4" s="1">
         <v>59.820520034625929</v>
       </c>
+      <c r="H4" s="2">
+        <v>50</v>
+      </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1621,6 +4399,9 @@
       <c r="G5" s="1">
         <v>41.464878088968575</v>
       </c>
+      <c r="H5" s="2">
+        <v>250</v>
+      </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1647,6 +4428,9 @@
       <c r="G6" s="1">
         <v>29.816405373772199</v>
       </c>
+      <c r="H6" s="2">
+        <v>500</v>
+      </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -1673,6 +4457,7 @@
       <c r="G7" s="1">
         <v>59.3</v>
       </c>
+      <c r="H7" s="2"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1699,6 +4484,9 @@
       <c r="G8" s="1">
         <v>59.69</v>
       </c>
+      <c r="H8" s="2">
+        <v>50</v>
+      </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1725,6 +4513,9 @@
       <c r="G9" s="1">
         <v>32.222548698019928</v>
       </c>
+      <c r="H9" s="2">
+        <v>250</v>
+      </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -1751,6 +4542,9 @@
       <c r="G10" s="1">
         <v>18.27795176331345</v>
       </c>
+      <c r="H10" s="2">
+        <v>500</v>
+      </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -1777,6 +4571,7 @@
       <c r="G11" s="1">
         <v>58.717355485937077</v>
       </c>
+      <c r="H11" s="2"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -1803,6 +4598,9 @@
       <c r="G12" s="1">
         <v>58.99475185998854</v>
       </c>
+      <c r="H12" s="2">
+        <v>100</v>
+      </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -1829,6 +4627,12 @@
       <c r="G13" s="1">
         <v>57.460614037571801</v>
       </c>
+      <c r="H13" s="2">
+        <v>100</v>
+      </c>
+      <c r="I13" s="1">
+        <v>225</v>
+      </c>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -1855,6 +4659,9 @@
       <c r="G14" s="1">
         <v>58.863545963581814</v>
       </c>
+      <c r="H14" s="2">
+        <v>100</v>
+      </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -1881,6 +4688,9 @@
       <c r="G15" s="1">
         <v>56.44</v>
       </c>
+      <c r="H15" s="2">
+        <v>100</v>
+      </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -1907,6 +4717,9 @@
       <c r="G16" s="1">
         <v>56.62</v>
       </c>
+      <c r="H16" s="2">
+        <v>100</v>
+      </c>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -1933,12 +4746,458 @@
       <c r="G17" s="1">
         <v>50.232844939073729</v>
       </c>
+      <c r="H17" s="2">
+        <v>100</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2500</v>
+      </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <f>'test 2D'!B3-'test 3D'!B3</f>
+        <v>1.9099999999999966</v>
+      </c>
+      <c r="C22" s="1">
+        <f>'test 2D'!C3-'test 3D'!C3</f>
+        <v>7.9999999999998295E-2</v>
+      </c>
+      <c r="D22" s="1">
+        <f>'test 2D'!D3-'test 3D'!D3</f>
+        <v>0.64999999999999858</v>
+      </c>
+      <c r="E22" s="1">
+        <f>'test 2D'!E3-'test 3D'!E3</f>
+        <v>0.19437168125591597</v>
+      </c>
+      <c r="F22" s="1">
+        <f>'test 2D'!F3-'test 3D'!F3</f>
+        <v>-1.7631972785712691</v>
+      </c>
+      <c r="G22" s="1">
+        <f>'test 2D'!G3-'test 3D'!G3</f>
+        <v>-0.52129675749787197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <f>'test 2D'!B4-'test 3D'!B4</f>
+        <v>-0.60000000000000142</v>
+      </c>
+      <c r="C23" s="1">
+        <f>'test 2D'!C4-'test 3D'!C4</f>
+        <v>-1.4500000000000028</v>
+      </c>
+      <c r="D23" s="1">
+        <f>'test 2D'!D4-'test 3D'!D4</f>
+        <v>-0.78999999999999915</v>
+      </c>
+      <c r="E23" s="1">
+        <f>'test 2D'!E4-'test 3D'!E4</f>
+        <v>-0.89346417363342567</v>
+      </c>
+      <c r="F23" s="1">
+        <f>'test 2D'!F4-'test 3D'!F4</f>
+        <v>-1.647703429493383</v>
+      </c>
+      <c r="G23" s="1">
+        <f>'test 2D'!G4-'test 3D'!G4</f>
+        <v>-2.6453525710801529</v>
+      </c>
+      <c r="H23" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <f>'test 2D'!B5-'test 3D'!B5</f>
+        <v>-4.2000000000000028</v>
+      </c>
+      <c r="C24" s="1">
+        <f>'test 2D'!C5-'test 3D'!C5</f>
+        <v>-0.25</v>
+      </c>
+      <c r="D24" s="1">
+        <f>'test 2D'!D5-'test 3D'!D5</f>
+        <v>-8.7700000000000031</v>
+      </c>
+      <c r="E24" s="1">
+        <f>'test 2D'!E5-'test 3D'!E5</f>
+        <v>-0.36183593891432508</v>
+      </c>
+      <c r="F24" s="1">
+        <f>'test 2D'!F5-'test 3D'!F5</f>
+        <v>-0.985732995172377</v>
+      </c>
+      <c r="G24" s="1">
+        <f>'test 2D'!G5-'test 3D'!G5</f>
+        <v>-2.0260051402627326</v>
+      </c>
+      <c r="H24" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <f>'test 2D'!B6-'test 3D'!B6</f>
+        <v>0.69999999999999929</v>
+      </c>
+      <c r="C25" s="1">
+        <f>'test 2D'!C6-'test 3D'!C6</f>
+        <v>0.30000000000000071</v>
+      </c>
+      <c r="D25" s="1">
+        <f>'test 2D'!D6-'test 3D'!D6</f>
+        <v>-1.4699999999999989</v>
+      </c>
+      <c r="E25" s="1">
+        <f>'test 2D'!E6-'test 3D'!E6</f>
+        <v>-3.5833581553526912</v>
+      </c>
+      <c r="F25" s="1">
+        <f>'test 2D'!F6-'test 3D'!F6</f>
+        <v>-1.0516182310616387</v>
+      </c>
+      <c r="G25" s="1">
+        <f>'test 2D'!G6-'test 3D'!G6</f>
+        <v>-4.9147222144532137</v>
+      </c>
+      <c r="H25" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <f>'test 2D'!B7-'test 3D'!B7</f>
+        <v>1.490000000000002</v>
+      </c>
+      <c r="C26" s="1">
+        <f>'test 2D'!C7-'test 3D'!C7</f>
+        <v>-0.14000000000000057</v>
+      </c>
+      <c r="D26" s="1">
+        <f>'test 2D'!D7-'test 3D'!D7</f>
+        <v>0.25999999999999801</v>
+      </c>
+      <c r="E26" s="1">
+        <f>'test 2D'!E7-'test 3D'!E7</f>
+        <v>0.56573603314166121</v>
+      </c>
+      <c r="F26" s="1">
+        <f>'test 2D'!F7-'test 3D'!F7</f>
+        <v>1.8405105919129028E-2</v>
+      </c>
+      <c r="G26" s="1">
+        <f>'test 2D'!G7-'test 3D'!G7</f>
+        <v>-0.66265507349084629</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <f>'test 2D'!B8-'test 3D'!B8</f>
+        <v>-1.1899999999999977</v>
+      </c>
+      <c r="C27" s="1">
+        <f>'test 2D'!C8-'test 3D'!C8</f>
+        <v>-1.2199999999999989</v>
+      </c>
+      <c r="D27" s="1">
+        <f>'test 2D'!D8-'test 3D'!D8</f>
+        <v>-0.81000000000000227</v>
+      </c>
+      <c r="E27" s="1">
+        <f>'test 2D'!E8-'test 3D'!E8</f>
+        <v>-1.4481699576085347</v>
+      </c>
+      <c r="F27" s="1">
+        <f>'test 2D'!F8-'test 3D'!F8</f>
+        <v>-0.68615128226476685</v>
+      </c>
+      <c r="G27" s="1">
+        <f>'test 2D'!G8-'test 3D'!G8</f>
+        <v>-0.9746497500343807</v>
+      </c>
+      <c r="H27" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <f>'test 2D'!B9-'test 3D'!B9</f>
+        <v>2.5399999999999991</v>
+      </c>
+      <c r="C28" s="1">
+        <f>'test 2D'!C9-'test 3D'!C9</f>
+        <v>3.6099999999999994</v>
+      </c>
+      <c r="D28" s="1">
+        <f>'test 2D'!D9-'test 3D'!D9</f>
+        <v>2.1099999999999994</v>
+      </c>
+      <c r="E28" s="1">
+        <f>'test 2D'!E9-'test 3D'!E9</f>
+        <v>-0.79504474814535797</v>
+      </c>
+      <c r="F28" s="1">
+        <f>'test 2D'!F9-'test 3D'!F9</f>
+        <v>-1.6703326216909602</v>
+      </c>
+      <c r="G28" s="1">
+        <f>'test 2D'!G9-'test 3D'!G9</f>
+        <v>-3.2799295639652897</v>
+      </c>
+      <c r="H28" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <f>'test 2D'!B10-'test 3D'!B10</f>
+        <v>1.6999999999999993</v>
+      </c>
+      <c r="C29" s="1">
+        <f>'test 2D'!C10-'test 3D'!C10</f>
+        <v>1.9399999999999995</v>
+      </c>
+      <c r="D29" s="1">
+        <f>'test 2D'!D10-'test 3D'!D10</f>
+        <v>3.66</v>
+      </c>
+      <c r="E29" s="1">
+        <f>'test 2D'!E10-'test 3D'!E10</f>
+        <v>-2.4467728867867748</v>
+      </c>
+      <c r="F29" s="1">
+        <f>'test 2D'!F10-'test 3D'!F10</f>
+        <v>-2.5933933051923717</v>
+      </c>
+      <c r="G29" s="1">
+        <f>'test 2D'!G10-'test 3D'!G10</f>
+        <v>-2.9260039479109636</v>
+      </c>
+      <c r="H29" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <f>'test 2D'!B11-'test 3D'!B11</f>
+        <v>-1.8400000000000034</v>
+      </c>
+      <c r="C30" s="1">
+        <f>'test 2D'!C11-'test 3D'!C11</f>
+        <v>0.78000000000000114</v>
+      </c>
+      <c r="D30" s="1">
+        <f>'test 2D'!D11-'test 3D'!D11</f>
+        <v>-1.2999999999999972</v>
+      </c>
+      <c r="E30" s="1">
+        <f>'test 2D'!E11-'test 3D'!E11</f>
+        <v>-1.9199497458146411</v>
+      </c>
+      <c r="F30" s="1">
+        <f>'test 2D'!F11-'test 3D'!F11</f>
+        <v>-1.4913736657309684</v>
+      </c>
+      <c r="G30" s="1">
+        <f>'test 2D'!G11-'test 3D'!G11</f>
+        <v>-0.93246978863556507</v>
+      </c>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <f>'test 2D'!B12-'test 3D'!B12</f>
+        <v>-1.0399999999999991</v>
+      </c>
+      <c r="C31" s="1">
+        <f>'test 2D'!C12-'test 3D'!C12</f>
+        <v>0.85000000000000142</v>
+      </c>
+      <c r="D31" s="1">
+        <f>'test 2D'!D12-'test 3D'!D12</f>
+        <v>-3</v>
+      </c>
+      <c r="E31" s="1">
+        <f>'test 2D'!E12-'test 3D'!E12</f>
+        <v>-0.98594598513748366</v>
+      </c>
+      <c r="F31" s="1">
+        <f>'test 2D'!F12-'test 3D'!F12</f>
+        <v>-0.21363257544603442</v>
+      </c>
+      <c r="G31" s="1">
+        <f>'test 2D'!G12-'test 3D'!G12</f>
+        <v>-1.466178083201001</v>
+      </c>
+      <c r="H31" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <f>'test 2D'!B13-'test 3D'!B13</f>
+        <v>-2.1300000000000026</v>
+      </c>
+      <c r="C32" s="1">
+        <f>'test 2D'!C13-'test 3D'!C13</f>
+        <v>0.64999999999999858</v>
+      </c>
+      <c r="D32" s="1">
+        <f>'test 2D'!D13-'test 3D'!D13</f>
+        <v>-2.5499999999999972</v>
+      </c>
+      <c r="E32" s="1">
+        <f>'test 2D'!E13-'test 3D'!E13</f>
+        <v>-0.86525987382162128</v>
+      </c>
+      <c r="F32" s="1">
+        <f>'test 2D'!F13-'test 3D'!F13</f>
+        <v>-0.70577081221260585</v>
+      </c>
+      <c r="G32" s="1">
+        <f>'test 2D'!G13-'test 3D'!G13</f>
+        <v>-0.17972569140657413</v>
+      </c>
+      <c r="H32" s="2">
+        <v>100</v>
+      </c>
+      <c r="I32" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <f>'test 2D'!B14-'test 3D'!B14</f>
+        <v>-1.8800000000000026</v>
+      </c>
+      <c r="C33" s="1">
+        <f>'test 2D'!C14-'test 3D'!C14</f>
+        <v>0.85000000000000142</v>
+      </c>
+      <c r="D33" s="1">
+        <f>'test 2D'!D14-'test 3D'!D14</f>
+        <v>-3.1000000000000014</v>
+      </c>
+      <c r="E33" s="1">
+        <f>'test 2D'!E14-'test 3D'!E14</f>
+        <v>-0.84404284511363414</v>
+      </c>
+      <c r="F33" s="1">
+        <f>'test 2D'!F14-'test 3D'!F14</f>
+        <v>-1.0235077908078694</v>
+      </c>
+      <c r="G33" s="1">
+        <f>'test 2D'!G14-'test 3D'!G14</f>
+        <v>-1.7922191257557643</v>
+      </c>
+      <c r="H33" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <f>'test 2D'!B15-'test 3D'!B15</f>
+        <v>-2.4799999999999969</v>
+      </c>
+      <c r="C34" s="1">
+        <f>'test 2D'!C15-'test 3D'!C15</f>
+        <v>0.77000000000000313</v>
+      </c>
+      <c r="D34" s="1">
+        <f>'test 2D'!D15-'test 3D'!D15</f>
+        <v>-3.6599999999999966</v>
+      </c>
+      <c r="E34" s="1">
+        <f>'test 2D'!E15-'test 3D'!E15</f>
+        <v>-0.78875647192840859</v>
+      </c>
+      <c r="F34" s="1">
+        <f>'test 2D'!F15-'test 3D'!F15</f>
+        <v>-0.43754785478162717</v>
+      </c>
+      <c r="G34" s="1">
+        <f>'test 2D'!G15-'test 3D'!G15</f>
+        <v>-3.4934899353366689E-2</v>
+      </c>
+      <c r="H34" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <f>'test 2D'!B16-'test 3D'!B16</f>
+        <v>-2.2800000000000011</v>
+      </c>
+      <c r="C35" s="1">
+        <f>'test 2D'!C16-'test 3D'!C16</f>
+        <v>1.5399999999999991</v>
+      </c>
+      <c r="D35" s="1">
+        <f>'test 2D'!D16-'test 3D'!D16</f>
+        <v>-2.9500000000000028</v>
+      </c>
+      <c r="E35" s="1">
+        <f>'test 2D'!E16-'test 3D'!E16</f>
+        <v>-0.43109180467887143</v>
+      </c>
+      <c r="F35" s="1">
+        <f>'test 2D'!F16-'test 3D'!F16</f>
+        <v>-2.3589387680772234E-2</v>
+      </c>
+      <c r="G35" s="1">
+        <f>'test 2D'!G16-'test 3D'!G16</f>
+        <v>-2.9547693339565342</v>
+      </c>
+      <c r="H35" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <f>'test 2D'!B17-'test 3D'!B17</f>
+        <v>-1.4399999999999977</v>
+      </c>
+      <c r="C36" s="1">
+        <f>'test 2D'!C17-'test 3D'!C17</f>
+        <v>2.2999999999999972</v>
+      </c>
+      <c r="D36" s="1">
+        <f>'test 2D'!D17-'test 3D'!D17</f>
+        <v>-0.35000000000000142</v>
+      </c>
+      <c r="E36" s="1">
+        <f>'test 2D'!E17-'test 3D'!E17</f>
+        <v>0.698070846558835</v>
+      </c>
+      <c r="F36" s="1">
+        <f>'test 2D'!F17-'test 3D'!F17</f>
+        <v>0.17549683686840467</v>
+      </c>
+      <c r="G36" s="1">
+        <f>'test 2D'!G17-'test 3D'!G17</f>
+        <v>-2.1493480161446783</v>
+      </c>
+      <c r="H36" s="2">
+        <v>100</v>
+      </c>
+      <c r="I36" s="1">
+        <v>2500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1946,56 +5205,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Zmieniono kolejnosc dzialow, dodano wykres FPS przy tworzeniu/niszczeniu, dopisano krotki cel
</commit_message>
<xml_diff>
--- a/doc/res/wynikiBenchmarkow.xlsx
+++ b/doc/res/wynikiBenchmarkow.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="test 2D" sheetId="1" r:id="rId1"/>
     <sheet name="test 3D" sheetId="2" r:id="rId2"/>
     <sheet name="test incrementalObjects" sheetId="3" r:id="rId3"/>
+    <sheet name="test creation-deletion" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t>Benchmark</t>
   </si>
@@ -483,11 +484,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153858816"/>
-        <c:axId val="153860736"/>
+        <c:axId val="154120960"/>
+        <c:axId val="154122880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153858816"/>
+        <c:axId val="154120960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,7 +517,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153860736"/>
+        <c:crossAx val="154122880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -524,7 +525,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153860736"/>
+        <c:axId val="154122880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,7 +562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153858816"/>
+        <c:crossAx val="154120960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -956,11 +957,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154569728"/>
-        <c:axId val="154580096"/>
+        <c:axId val="154831872"/>
+        <c:axId val="154842240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154569728"/>
+        <c:axId val="154831872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -996,7 +997,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154580096"/>
+        <c:crossAx val="154842240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1004,7 +1005,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154580096"/>
+        <c:axId val="154842240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1034,7 +1035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154569728"/>
+        <c:crossAx val="154831872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1402,11 +1403,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154678784"/>
-        <c:axId val="154680704"/>
+        <c:axId val="154940928"/>
+        <c:axId val="154942848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154678784"/>
+        <c:axId val="154940928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1447,7 +1448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154680704"/>
+        <c:crossAx val="154942848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1455,7 +1456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154680704"/>
+        <c:axId val="154942848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -1493,7 +1494,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154678784"/>
+        <c:crossAx val="154940928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1893,11 +1894,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="90826240"/>
-        <c:axId val="90915200"/>
+        <c:axId val="155047808"/>
+        <c:axId val="155062272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90826240"/>
+        <c:axId val="155047808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1926,7 +1927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90915200"/>
+        <c:crossAx val="155062272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1934,7 +1935,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90915200"/>
+        <c:axId val="155062272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1964,7 +1965,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90826240"/>
+        <c:crossAx val="155047808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2373,11 +2374,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="91073920"/>
-        <c:axId val="89769088"/>
+        <c:axId val="155099904"/>
+        <c:axId val="155101824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91073920"/>
+        <c:axId val="155099904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2406,7 +2407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89769088"/>
+        <c:crossAx val="155101824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2414,7 +2415,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89769088"/>
+        <c:axId val="155101824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2444,7 +2445,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91073920"/>
+        <c:crossAx val="155099904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3105,11 +3106,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="154780032"/>
-        <c:axId val="154781568"/>
+        <c:axId val="153865600"/>
+        <c:axId val="153871872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="154780032"/>
+        <c:axId val="153865600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3155,7 +3156,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154781568"/>
+        <c:crossAx val="153871872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3163,7 +3164,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154781568"/>
+        <c:axId val="153871872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3200,7 +3201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154780032"/>
+        <c:crossAx val="153865600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3217,6 +3218,356 @@
           <c:h val="0.50230314960629918"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200"/>
+              <a:t>Stabilna</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+              <a:t> ilość obiektów tworzona na klatkę</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL" sz="1200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test creation-deletion'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$H$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test creation-deletion'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$H$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test creation-deletion'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$H$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test creation-deletion'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$H$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test creation-deletion'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$H$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'test creation-deletion'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$H$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'test creation-deletion'!$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="43981056"/>
+        <c:axId val="43982848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="43981056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43982848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43982848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Ilość obiektów na klatkę</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43981056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3407,6 +3758,41 @@
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3718,7 +4104,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4288,7 +4674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -5513,4 +5899,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>70</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>75</v>
+      </c>
+      <c r="E2">
+        <v>140</v>
+      </c>
+      <c r="F2">
+        <v>115</v>
+      </c>
+      <c r="G2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Dodano diagarmy dla gry dwuwymiarowej w zasobach i wykresy do wnioskow dla obu gier, wprowadzono poprawki w kursywie, kropkach, ujednolicono styl, zlikwidowano jednozdaniowe akapity
</commit_message>
<xml_diff>
--- a/doc/res/wynikiBenchmarkow.xlsx
+++ b/doc/res/wynikiBenchmarkow.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="test 2D" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,15 @@
     <sheet name="test incrementalObjects" sheetId="3" r:id="rId3"/>
     <sheet name="test creation-deletion" sheetId="4" r:id="rId4"/>
     <sheet name="gartner" sheetId="5" r:id="rId5"/>
+    <sheet name="2d" sheetId="6" r:id="rId6"/>
+    <sheet name="3d" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
   <si>
     <t>Benchmark</t>
   </si>
@@ -74,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,7 +113,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -125,7 +127,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -153,6 +165,7 @@
       </c:layout>
       <c:overlay val="1"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -168,6 +181,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -182,6 +196,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$4:$I$6</c:f>
@@ -233,6 +248,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$4:$I$6</c:f>
@@ -284,6 +300,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$4:$I$6</c:f>
@@ -335,6 +352,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$4:$I$6</c:f>
@@ -386,6 +404,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$4:$I$6</c:f>
@@ -437,6 +456,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$4:$I$6</c:f>
@@ -474,15 +494,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="74937472"/>
-        <c:axId val="74939392"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="154476928"/>
+        <c:axId val="154478848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74937472"/>
+        <c:axId val="154476928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -500,20 +529,26 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74939392"/>
+        <c:crossAx val="154478848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74939392"/>
+        <c:axId val="154478848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -540,19 +575,25 @@
               <c:y val="0.49170312044327785"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74937472"/>
+        <c:crossAx val="154476928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -562,9 +603,777 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="81613568"/>
+        <c:axId val="81615104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="81613568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81615104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="81615104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81613568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="80900480"/>
+        <c:axId val="80902016"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="80900480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80902016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="80902016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80900480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3d'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'3d'!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3d'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'3d'!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3d'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'3d'!$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.13</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3d'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'3d'!$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3d'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'3d'!$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3d'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'3d'!$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="90717568"/>
+        <c:axId val="176682112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90717568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="176682112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="176682112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90717568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -595,12 +1404,15 @@
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -615,6 +1427,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$8:$I$10</c:f>
@@ -666,6 +1479,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$8:$I$10</c:f>
@@ -717,6 +1531,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$8:$I$10</c:f>
@@ -768,6 +1583,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$8:$I$10</c:f>
@@ -819,6 +1635,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$8:$I$10</c:f>
@@ -870,6 +1687,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 2D'!$I$8:$I$10</c:f>
@@ -907,15 +1725,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="76125696"/>
-        <c:axId val="76127616"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="154612864"/>
+        <c:axId val="154614784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76125696"/>
+        <c:axId val="154612864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -941,20 +1768,25 @@
               <c:y val="0.92960629921259852"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76127616"/>
+        <c:crossAx val="154614784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76127616"/>
+        <c:axId val="154614784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -973,19 +1805,26 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76125696"/>
+        <c:crossAx val="154612864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -997,7 +1836,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1027,7 +1876,9 @@
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1043,6 +1894,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1057,6 +1909,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
@@ -1102,6 +1955,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
@@ -1147,6 +2001,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
@@ -1192,6 +2047,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
@@ -1237,6 +2093,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
@@ -1282,6 +2139,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>('test 2D'!$J$13,'test 2D'!$J$17)</c:f>
@@ -1313,15 +2171,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="75028352"/>
-        <c:axId val="76152832"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="154683264"/>
+        <c:axId val="154701824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75028352"/>
+        <c:axId val="154683264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1352,21 +2219,26 @@
               <c:y val="0.92960629921259852"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76152832"/>
+        <c:crossAx val="154701824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76152832"/>
+        <c:axId val="154701824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1393,19 +2265,25 @@
               <c:y val="0.45951552930883638"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75028352"/>
+        <c:crossAx val="154683264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1417,7 +2295,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1443,7 +2331,9 @@
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1459,6 +2349,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1473,6 +2364,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -1524,6 +2416,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -1575,6 +2468,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -1626,6 +2520,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -1677,6 +2572,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -1728,6 +2624,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -1765,15 +2662,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="76528256"/>
-        <c:axId val="76538624"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="154782720"/>
+        <c:axId val="154797184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76528256"/>
+        <c:axId val="154782720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1791,20 +2697,26 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76538624"/>
+        <c:crossAx val="154797184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76538624"/>
+        <c:axId val="154797184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1823,10 +2735,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76528256"/>
+        <c:crossAx val="154782720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1843,9 +2759,11 @@
           <c:h val="0.50230314960629907"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1857,7 +2775,17 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1883,7 +2811,9 @@
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1899,6 +2829,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1913,6 +2844,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -1964,6 +2896,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -2015,6 +2948,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -2066,6 +3000,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -2117,6 +3052,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -2168,6 +3104,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test 3D'!$H$4:$H$6</c:f>
@@ -2205,15 +3142,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="76598272"/>
-        <c:axId val="76612736"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="153437696"/>
+        <c:axId val="153439616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76598272"/>
+        <c:axId val="153437696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2231,20 +3177,26 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76612736"/>
+        <c:crossAx val="153439616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76612736"/>
+        <c:axId val="153439616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2263,10 +3215,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76598272"/>
+        <c:crossAx val="153437696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2283,9 +3239,11 @@
           <c:h val="0.50230314960629907"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2297,7 +3255,17 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2323,7 +3291,9 @@
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2338,6 +3308,7 @@
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2430,6 +3401,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2523,6 +3495,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2616,6 +3589,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2709,6 +3683,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -2802,6 +3777,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -2895,17 +3871,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="86930560"/>
-        <c:axId val="86932480"/>
+        <c:smooth val="0"/>
+        <c:axId val="153576576"/>
+        <c:axId val="153578496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="86930560"/>
+        <c:axId val="153576576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2931,8 +3917,11 @@
               <c:y val="0.92960629921259852"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="2700000"/>
@@ -2941,20 +3930,22 @@
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86932480"/>
+        <c:crossAx val="153578496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86932480"/>
+        <c:axId val="153578496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2981,10 +3972,13 @@
               <c:y val="0.4006838728492273"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86930560"/>
+        <c:crossAx val="153576576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3001,9 +3995,11 @@
           <c:h val="0.50230314960629907"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3015,7 +4011,17 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3039,12 +4045,15 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3059,6 +4068,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test creation-deletion'!$H$1</c:f>
@@ -3095,6 +4105,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test creation-deletion'!$H$1</c:f>
@@ -3131,6 +4142,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test creation-deletion'!$H$1</c:f>
@@ -3167,6 +4179,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test creation-deletion'!$H$1</c:f>
@@ -3203,6 +4216,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test creation-deletion'!$H$1</c:f>
@@ -3239,6 +4253,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'test creation-deletion'!$H$1</c:f>
@@ -3261,29 +4276,42 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="86987136"/>
-        <c:axId val="86988672"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="154871680"/>
+        <c:axId val="154873216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86987136"/>
+        <c:axId val="154871680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86988672"/>
+        <c:crossAx val="154873216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86988672"/>
+        <c:axId val="154873216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -3303,10 +4331,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86987136"/>
+        <c:crossAx val="154871680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3314,9 +4345,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3328,7 +4361,17 @@
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3352,7 +4395,9 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -3361,7 +4406,12 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:dLbls>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
           </c:dLbls>
           <c:cat>
@@ -3412,14 +4462,278 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>54.76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>36.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>47.21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPhone 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>59.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>57.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2d'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>iPad 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'2d'!$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>40.229999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="73619328"/>
+        <c:axId val="73620864"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="73619328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73620864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="73620864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="73619328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3696,10 +5010,140 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3737,7 +5181,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3771,6 +5215,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3805,9 +5250,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3980,14 +5426,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -3996,7 +5442,7 @@
     <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -4025,12 +5471,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4056,7 +5502,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4085,7 +5531,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4114,7 +5560,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4143,7 +5589,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4170,7 +5616,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4199,7 +5645,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4228,7 +5674,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4257,7 +5703,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4284,7 +5730,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4313,7 +5759,7 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4345,7 +5791,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4374,7 +5820,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4403,7 +5849,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4432,7 +5878,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4464,12 +5910,12 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <f>B4-B8</f>
         <v>0.58999999999999631</v>
@@ -4492,7 +5938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <f t="shared" ref="B26:G27" si="1">B5-B9</f>
         <v>12.259999999999998</v>
@@ -4518,7 +5964,7 @@
         <v>10.496253814651205</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -4551,16 +5997,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -4583,12 +6029,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4614,7 +6060,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4643,7 +6089,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4672,7 +6118,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4701,7 +6147,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4728,7 +6174,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4757,7 +6203,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4786,7 +6232,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4815,7 +6261,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4842,7 +6288,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4871,7 +6317,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4903,7 +6349,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4932,7 +6378,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4961,7 +6407,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4990,7 +6436,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5022,12 +6468,12 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <f>'test 2D'!B3-'test 3D'!B3</f>
         <v>1.9099999999999966</v>
@@ -5053,7 +6499,7 @@
         <v>-0.52129675749787197</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <f>'test 2D'!B4-'test 3D'!B4</f>
         <v>-0.60000000000000142</v>
@@ -5082,7 +6528,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <f>'test 2D'!B5-'test 3D'!B5</f>
         <v>-4.2000000000000028</v>
@@ -5111,7 +6557,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <f>'test 2D'!B6-'test 3D'!B6</f>
         <v>0.69999999999999929</v>
@@ -5140,7 +6586,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <f>'test 2D'!B7-'test 3D'!B7</f>
         <v>1.490000000000002</v>
@@ -5167,7 +6613,7 @@
       </c>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <f>'test 2D'!B8-'test 3D'!B8</f>
         <v>-1.1899999999999977</v>
@@ -5196,7 +6642,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <f>'test 2D'!B9-'test 3D'!B9</f>
         <v>2.5399999999999991</v>
@@ -5225,7 +6671,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <f>'test 2D'!B10-'test 3D'!B10</f>
         <v>1.6999999999999993</v>
@@ -5254,7 +6700,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <f>'test 2D'!B11-'test 3D'!B11</f>
         <v>-1.8400000000000034</v>
@@ -5281,7 +6727,7 @@
       </c>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <f>'test 2D'!B12-'test 3D'!B12</f>
         <v>-1.0399999999999991</v>
@@ -5310,7 +6756,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <f>'test 2D'!B13-'test 3D'!B13</f>
         <v>-2.1300000000000026</v>
@@ -5342,7 +6788,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <f>'test 2D'!B14-'test 3D'!B14</f>
         <v>-1.8800000000000026</v>
@@ -5371,7 +6817,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <f>'test 2D'!B15-'test 3D'!B15</f>
         <v>-2.4799999999999969</v>
@@ -5400,7 +6846,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <f>'test 2D'!B16-'test 3D'!B16</f>
         <v>-2.2800000000000011</v>
@@ -5429,7 +6875,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <f>'test 2D'!B17-'test 3D'!B17</f>
         <v>-1.4399999999999977</v>
@@ -5468,16 +6914,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5500,12 +6946,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>50</v>
       </c>
@@ -5528,7 +6974,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100</v>
       </c>
@@ -5551,7 +6997,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>250</v>
       </c>
@@ -5574,7 +7020,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>500</v>
       </c>
@@ -5597,7 +7043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>750</v>
       </c>
@@ -5620,7 +7066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -5643,7 +7089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1250</v>
       </c>
@@ -5666,7 +7112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1500</v>
       </c>
@@ -5689,7 +7135,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1750</v>
       </c>
@@ -5712,7 +7158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2000</v>
       </c>
@@ -5735,7 +7181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -5743,7 +7189,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -5751,7 +7197,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -5759,7 +7205,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -5767,7 +7213,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -5782,16 +7228,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -5814,7 +7260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>70</v>
       </c>
@@ -5834,7 +7280,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -5842,7 +7288,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -5850,7 +7296,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -5858,7 +7304,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -5866,7 +7312,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -5874,7 +7320,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -5882,7 +7328,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -5890,7 +7336,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -5898,7 +7344,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -5906,7 +7352,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -5914,7 +7360,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -5922,7 +7368,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -5930,7 +7376,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -5938,7 +7384,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -5946,7 +7392,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -5961,16 +7407,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -5978,7 +7424,7 @@
         <v>78.400000000000006</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -5986,7 +7432,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -5994,7 +7440,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
@@ -6002,7 +7448,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -6010,14 +7456,165 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C9">
         <f>SUM(C3:C7)</f>
         <v>100.00000000000001</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>59.88</v>
+      </c>
+      <c r="C3">
+        <v>59.34</v>
+      </c>
+      <c r="D3">
+        <v>59.88</v>
+      </c>
+      <c r="E3">
+        <v>59.97</v>
+      </c>
+      <c r="F3">
+        <v>59.88</v>
+      </c>
+      <c r="G3">
+        <v>59.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>54.76</v>
+      </c>
+      <c r="C4" s="1">
+        <v>36.6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>47.21</v>
+      </c>
+      <c r="E4" s="1">
+        <v>59.65</v>
+      </c>
+      <c r="F4" s="1">
+        <v>57.5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>40.229999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>59.67</v>
+      </c>
+      <c r="C3">
+        <v>59.06</v>
+      </c>
+      <c r="D3">
+        <v>59.13</v>
+      </c>
+      <c r="E3" s="1">
+        <v>59.75</v>
+      </c>
+      <c r="F3" s="1">
+        <v>59.83</v>
+      </c>
+      <c r="G3" s="1">
+        <v>59.47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>